<commit_message>
some refactoring of names and add dump low coverage results to file
</commit_message>
<xml_diff>
--- a/coverage.xlsx
+++ b/coverage.xlsx
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>0.9999999999900399</v>
@@ -594,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
         <v>0.99999999999</v>
@@ -649,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>0.99999999999002</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>0.9999999999900497</v>
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>0.999999999989605</v>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
         <v>0.3181818181786741</v>
@@ -869,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
         <v>0.6666666666600133</v>
@@ -922,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
         <v>0.9229979466024333</v>
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
         <v>0.8065476190396176</v>
@@ -1024,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>0.3004975124348209</v>
@@ -1075,7 +1075,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>0.7440239043750595</v>
@@ -1126,7 +1126,7 @@
         <v>0.15</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>0.08901734103943333</v>
@@ -1174,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
         <v>0.99999999999002</v>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>0.9999999999893617</v>
@@ -1275,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>0.9999999999889257</v>
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
         <v>0.633100697899969</v>
@@ -1385,7 +1385,7 @@
         <v>0.9</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0999999999</v>
+        <v>0.9000000001</v>
       </c>
       <c r="H18" t="n">
         <v>0.9764705882123184</v>
@@ -1441,7 +1441,7 @@
         <v>0.86</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1666666663888889</v>
+        <v>0.8333333336111111</v>
       </c>
       <c r="H19" t="n">
         <v>0.9441517386623377</v>
@@ -1495,7 +1495,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
         <v>0.02314814814707647</v>
@@ -1549,7 +1549,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>0.4573643410764077</v>

</xml_diff>